<commit_message>
migrated from sqlite to postgresql
</commit_message>
<xml_diff>
--- a/temp_task_files/file.xlsx
+++ b/temp_task_files/file.xlsx
@@ -16,7 +16,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -28,7 +28,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -45,9 +45,9 @@
         <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -75,14 +75,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -110,6 +127,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -254,7 +288,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>